<commit_message>
Add objective function and calibrate script
</commit_message>
<xml_diff>
--- a/data/DOERefBuildings/BLD10.xlsx
+++ b/data/DOERefBuildings/BLD10.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maoj\Dropbox\UWG_Matlab-master\data\DOERefBuildings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\UWG\data\DOERefBuildings\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="491505" yWindow="135" windowWidth="19320" windowHeight="11640" tabRatio="724" activeTab="1"/>
+    <workbookView xWindow="471090" yWindow="135" windowWidth="19320" windowHeight="11640" tabRatio="724" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="70" r:id="rId1"/>
@@ -4273,8 +4273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
@@ -4419,7 +4419,7 @@
         <v>10</v>
       </c>
       <c r="N3" s="84">
-        <v>13.47828054</v>
+        <v>13.331091536182738</v>
       </c>
       <c r="O3" s="84">
         <v>12.341784891792569</v>
@@ -4477,7 +4477,7 @@
       </c>
       <c r="N4" s="84">
         <f>$N$3</f>
-        <v>13.47828054</v>
+        <v>13.331091536182738</v>
       </c>
       <c r="O4" s="84">
         <v>12.341784891792569</v>
@@ -4537,7 +4537,7 @@
       </c>
       <c r="N5" s="84">
         <f>$N$3</f>
-        <v>13.47828054</v>
+        <v>13.331091536182738</v>
       </c>
       <c r="O5" s="84">
         <v>12.341784891792569</v>
@@ -6963,7 +6963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG43"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -7936,99 +7936,99 @@
         <v>181</v>
       </c>
       <c r="G11" s="48">
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="H11" s="48">
         <f>$G$11</f>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="I11" s="48">
         <f t="shared" ref="I11:AD13" si="0">$G$11</f>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="J11" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="K11" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="L11" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="M11" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="N11" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="O11" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="P11" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Q11" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="R11" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="S11" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="T11" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="U11" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="V11" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="W11" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="X11" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Y11" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Z11" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AA11" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AB11" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AC11" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AD11" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AE11" s="48">
         <v>576</v>
@@ -8053,99 +8053,99 @@
       </c>
       <c r="G12" s="48">
         <f>$G$11</f>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="H12" s="48">
         <f t="shared" ref="H12" si="1">$G$11</f>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="I12" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="J12" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="K12" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="L12" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="M12" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="N12" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="O12" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="P12" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Q12" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="R12" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="S12" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="T12" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="U12" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="V12" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="W12" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="X12" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Y12" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Z12" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AA12" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AB12" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AC12" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AD12" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AE12" s="48">
         <v>648</v>
@@ -8166,99 +8166,99 @@
       </c>
       <c r="G13" s="48">
         <f t="shared" ref="G13:V16" si="2">$G$11</f>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="H13" s="48">
         <f t="shared" si="2"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="I13" s="48">
         <f t="shared" si="2"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="J13" s="48">
         <f t="shared" si="2"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="K13" s="48">
         <f t="shared" si="2"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="L13" s="48">
         <f t="shared" si="2"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="M13" s="48">
         <f t="shared" si="2"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="N13" s="48">
         <f t="shared" si="2"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="O13" s="48">
         <f t="shared" si="2"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="P13" s="48">
         <f t="shared" si="2"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Q13" s="48">
         <f t="shared" si="2"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="R13" s="48">
         <f t="shared" si="2"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="S13" s="48">
         <f t="shared" si="2"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="T13" s="48">
         <f t="shared" si="2"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="U13" s="48">
         <f t="shared" si="2"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="V13" s="48">
         <f t="shared" si="2"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="W13" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="X13" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Y13" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Z13" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AA13" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AB13" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AC13" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AD13" s="48">
         <f t="shared" si="0"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AE13" s="48"/>
       <c r="AF13" s="48"/>
@@ -8285,99 +8285,99 @@
       </c>
       <c r="G14" s="48">
         <f t="shared" si="2"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="H14" s="48">
         <f t="shared" ref="H14:AD16" si="3">$G$11</f>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="I14" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="J14" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="K14" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="L14" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="M14" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="N14" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="O14" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="P14" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Q14" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="R14" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="S14" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="T14" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="U14" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="V14" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="W14" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="X14" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Y14" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Z14" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AA14" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AB14" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AC14" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AD14" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AE14" s="48">
         <v>504</v>
@@ -8402,99 +8402,99 @@
       </c>
       <c r="G15" s="48">
         <f t="shared" si="2"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="H15" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="I15" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="J15" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="K15" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="L15" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="M15" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="N15" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="O15" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="P15" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Q15" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="R15" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="S15" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="T15" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="U15" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="V15" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="W15" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="X15" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Y15" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Z15" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AA15" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AB15" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AC15" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AD15" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AE15" s="48">
         <v>384</v>
@@ -8515,99 +8515,99 @@
       </c>
       <c r="G16" s="48">
         <f t="shared" si="2"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="H16" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="I16" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="J16" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="K16" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="L16" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="M16" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="N16" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="O16" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="P16" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Q16" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="R16" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="S16" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="T16" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="U16" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="V16" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="W16" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="X16" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Y16" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Z16" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AA16" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AB16" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AC16" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AD16" s="48">
         <f t="shared" si="3"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AE16" s="48">
         <v>384</v>
@@ -10015,99 +10015,99 @@
       </c>
       <c r="G32" s="48">
         <f>$G$11</f>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="H32" s="48">
         <f t="shared" ref="H32:AD37" si="4">$G$11</f>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="I32" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="J32" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="K32" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="L32" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="M32" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="N32" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="O32" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="P32" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Q32" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="R32" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="S32" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="T32" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="U32" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="V32" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="W32" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="X32" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Y32" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Z32" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AA32" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AB32" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AC32" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AD32" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AE32" s="48">
         <v>576</v>
@@ -10130,99 +10130,99 @@
       </c>
       <c r="G33" s="48">
         <f t="shared" ref="G33:G37" si="5">$G$11</f>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="H33" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="I33" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="J33" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="K33" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="L33" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="M33" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="N33" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="O33" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="P33" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Q33" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="R33" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="S33" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="T33" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="U33" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="V33" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="W33" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="X33" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Y33" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Z33" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AA33" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AB33" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AC33" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AD33" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AE33" s="48">
         <v>648</v>
@@ -10243,99 +10243,99 @@
       </c>
       <c r="G34" s="48">
         <f t="shared" si="5"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="H34" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="I34" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="J34" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="K34" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="L34" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="M34" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="N34" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="O34" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="P34" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Q34" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="R34" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="S34" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="T34" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="U34" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="V34" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="W34" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="X34" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Y34" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Z34" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AA34" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AB34" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AC34" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AD34" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AE34" s="48">
         <v>648</v>
@@ -10364,99 +10364,99 @@
       </c>
       <c r="G35" s="48">
         <f t="shared" si="5"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="H35" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="I35" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="J35" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="K35" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="L35" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="M35" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="N35" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="O35" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="P35" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Q35" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="R35" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="S35" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="T35" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="U35" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="V35" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="W35" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="X35" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Y35" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Z35" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AA35" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AB35" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AC35" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AD35" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AE35" s="48">
         <v>504</v>
@@ -10479,99 +10479,99 @@
       </c>
       <c r="G36" s="48">
         <f t="shared" si="5"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="H36" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="I36" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="J36" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="K36" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="L36" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="M36" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="N36" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="O36" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="P36" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Q36" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="R36" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="S36" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="T36" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="U36" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="V36" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="W36" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="X36" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Y36" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Z36" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AA36" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AB36" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AC36" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AD36" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AE36" s="48">
         <v>384</v>
@@ -10592,99 +10592,99 @@
       </c>
       <c r="G37" s="48">
         <f t="shared" si="5"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="H37" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="I37" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="J37" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="K37" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="L37" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="M37" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="N37" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="O37" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="P37" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Q37" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="R37" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="S37" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="T37" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="U37" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="V37" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="W37" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="X37" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Y37" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="Z37" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AA37" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AB37" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AC37" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AD37" s="48">
         <f t="shared" si="4"/>
-        <v>20.112982349999999</v>
+        <v>22.005069812337766</v>
       </c>
       <c r="AE37" s="48">
         <v>384</v>

</xml_diff>

<commit_message>
Improve codes to decrease simulation time in optimziation
</commit_message>
<xml_diff>
--- a/data/DOERefBuildings/BLD10.xlsx
+++ b/data/DOERefBuildings/BLD10.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="471090" yWindow="135" windowWidth="19320" windowHeight="11640" tabRatio="724" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="471090" yWindow="135" windowWidth="19320" windowHeight="11640" tabRatio="724" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="70" r:id="rId1"/>
@@ -4273,7 +4273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="L1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
@@ -4419,7 +4419,7 @@
         <v>10</v>
       </c>
       <c r="N3" s="84">
-        <v>13.331091536182738</v>
+        <v>13</v>
       </c>
       <c r="O3" s="84">
         <v>12.341784891792569</v>
@@ -4477,7 +4477,7 @@
       </c>
       <c r="N4" s="84">
         <f>$N$3</f>
-        <v>13.331091536182738</v>
+        <v>13</v>
       </c>
       <c r="O4" s="84">
         <v>12.341784891792569</v>
@@ -4537,7 +4537,7 @@
       </c>
       <c r="N5" s="84">
         <f>$N$3</f>
-        <v>13.331091536182738</v>
+        <v>13</v>
       </c>
       <c r="O5" s="84">
         <v>12.341784891792569</v>
@@ -6963,7 +6963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG43"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -7936,99 +7936,99 @@
         <v>181</v>
       </c>
       <c r="G11" s="48">
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="H11" s="48">
         <f>$G$11</f>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="I11" s="48">
         <f t="shared" ref="I11:AD13" si="0">$G$11</f>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="J11" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="K11" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="L11" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="M11" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="N11" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="O11" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="P11" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Q11" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="R11" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="S11" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="T11" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="U11" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="V11" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="W11" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="X11" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Y11" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Z11" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AA11" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AB11" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AC11" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AD11" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AE11" s="48">
         <v>576</v>
@@ -8053,99 +8053,99 @@
       </c>
       <c r="G12" s="48">
         <f>$G$11</f>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="H12" s="48">
         <f t="shared" ref="H12" si="1">$G$11</f>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="I12" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="J12" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="K12" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="L12" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="M12" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="N12" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="O12" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="P12" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Q12" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="R12" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="S12" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="T12" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="U12" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="V12" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="W12" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="X12" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Y12" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Z12" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AA12" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AB12" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AC12" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AD12" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AE12" s="48">
         <v>648</v>
@@ -8166,99 +8166,99 @@
       </c>
       <c r="G13" s="48">
         <f t="shared" ref="G13:V16" si="2">$G$11</f>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="H13" s="48">
         <f t="shared" si="2"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="I13" s="48">
         <f t="shared" si="2"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="J13" s="48">
         <f t="shared" si="2"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="K13" s="48">
         <f t="shared" si="2"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="L13" s="48">
         <f t="shared" si="2"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="M13" s="48">
         <f t="shared" si="2"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="N13" s="48">
         <f t="shared" si="2"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="O13" s="48">
         <f t="shared" si="2"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="P13" s="48">
         <f t="shared" si="2"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Q13" s="48">
         <f t="shared" si="2"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="R13" s="48">
         <f t="shared" si="2"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="S13" s="48">
         <f t="shared" si="2"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="T13" s="48">
         <f t="shared" si="2"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="U13" s="48">
         <f t="shared" si="2"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="V13" s="48">
         <f t="shared" si="2"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="W13" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="X13" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Y13" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Z13" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AA13" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AB13" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AC13" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AD13" s="48">
         <f t="shared" si="0"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AE13" s="48"/>
       <c r="AF13" s="48"/>
@@ -8285,99 +8285,99 @@
       </c>
       <c r="G14" s="48">
         <f t="shared" si="2"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="H14" s="48">
         <f t="shared" ref="H14:AD16" si="3">$G$11</f>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="I14" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="J14" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="K14" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="L14" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="M14" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="N14" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="O14" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="P14" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Q14" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="R14" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="S14" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="T14" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="U14" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="V14" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="W14" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="X14" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Y14" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Z14" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AA14" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AB14" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AC14" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AD14" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AE14" s="48">
         <v>504</v>
@@ -8402,99 +8402,99 @@
       </c>
       <c r="G15" s="48">
         <f t="shared" si="2"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="H15" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="I15" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="J15" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="K15" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="L15" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="M15" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="N15" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="O15" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="P15" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Q15" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="R15" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="S15" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="T15" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="U15" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="V15" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="W15" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="X15" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Y15" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Z15" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AA15" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AB15" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AC15" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AD15" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AE15" s="48">
         <v>384</v>
@@ -8515,99 +8515,99 @@
       </c>
       <c r="G16" s="48">
         <f t="shared" si="2"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="H16" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="I16" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="J16" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="K16" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="L16" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="M16" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="N16" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="O16" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="P16" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Q16" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="R16" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="S16" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="T16" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="U16" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="V16" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="W16" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="X16" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Y16" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Z16" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AA16" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AB16" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AC16" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AD16" s="48">
         <f t="shared" si="3"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AE16" s="48">
         <v>384</v>
@@ -10015,99 +10015,99 @@
       </c>
       <c r="G32" s="48">
         <f>$G$11</f>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="H32" s="48">
         <f t="shared" ref="H32:AD37" si="4">$G$11</f>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="I32" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="J32" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="K32" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="L32" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="M32" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="N32" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="O32" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="P32" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Q32" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="R32" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="S32" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="T32" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="U32" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="V32" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="W32" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="X32" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Y32" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Z32" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AA32" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AB32" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AC32" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AD32" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AE32" s="48">
         <v>576</v>
@@ -10130,99 +10130,99 @@
       </c>
       <c r="G33" s="48">
         <f t="shared" ref="G33:G37" si="5">$G$11</f>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="H33" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="I33" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="J33" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="K33" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="L33" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="M33" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="N33" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="O33" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="P33" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Q33" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="R33" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="S33" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="T33" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="U33" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="V33" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="W33" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="X33" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Y33" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Z33" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AA33" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AB33" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AC33" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AD33" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AE33" s="48">
         <v>648</v>
@@ -10243,99 +10243,99 @@
       </c>
       <c r="G34" s="48">
         <f t="shared" si="5"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="H34" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="I34" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="J34" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="K34" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="L34" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="M34" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="N34" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="O34" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="P34" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Q34" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="R34" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="S34" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="T34" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="U34" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="V34" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="W34" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="X34" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Y34" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Z34" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AA34" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AB34" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AC34" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AD34" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AE34" s="48">
         <v>648</v>
@@ -10364,99 +10364,99 @@
       </c>
       <c r="G35" s="48">
         <f t="shared" si="5"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="H35" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="I35" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="J35" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="K35" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="L35" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="M35" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="N35" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="O35" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="P35" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Q35" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="R35" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="S35" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="T35" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="U35" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="V35" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="W35" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="X35" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Y35" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Z35" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AA35" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AB35" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AC35" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AD35" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AE35" s="48">
         <v>504</v>
@@ -10479,99 +10479,99 @@
       </c>
       <c r="G36" s="48">
         <f t="shared" si="5"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="H36" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="I36" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="J36" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="K36" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="L36" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="M36" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="N36" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="O36" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="P36" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Q36" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="R36" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="S36" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="T36" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="U36" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="V36" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="W36" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="X36" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Y36" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Z36" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AA36" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AB36" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AC36" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AD36" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AE36" s="48">
         <v>384</v>
@@ -10592,99 +10592,99 @@
       </c>
       <c r="G37" s="48">
         <f t="shared" si="5"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="H37" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="I37" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="J37" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="K37" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="L37" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="M37" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="N37" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="O37" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="P37" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Q37" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="R37" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="S37" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="T37" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="U37" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="V37" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="W37" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="X37" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Y37" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="Z37" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AA37" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AB37" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AC37" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AD37" s="48">
         <f t="shared" si="4"/>
-        <v>22.005069812337766</v>
+        <v>22</v>
       </c>
       <c r="AE37" s="48">
         <v>384</v>

</xml_diff>

<commit_message>
Add backprogation ANN model in surrogate
</commit_message>
<xml_diff>
--- a/data/DOERefBuildings/BLD10.xlsx
+++ b/data/DOERefBuildings/BLD10.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="471090" yWindow="135" windowWidth="19320" windowHeight="11640" tabRatio="724" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="471090" yWindow="135" windowWidth="19320" windowHeight="11640" tabRatio="724" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="70" r:id="rId1"/>
@@ -4273,7 +4273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
@@ -4419,7 +4419,7 @@
         <v>10</v>
       </c>
       <c r="N3" s="84">
-        <v>13</v>
+        <v>12.4789124008953</v>
       </c>
       <c r="O3" s="84">
         <v>12.341784891792569</v>
@@ -4477,7 +4477,7 @@
       </c>
       <c r="N4" s="84">
         <f>$N$3</f>
-        <v>13</v>
+        <v>12.4789124008953</v>
       </c>
       <c r="O4" s="84">
         <v>12.341784891792569</v>
@@ -4537,7 +4537,7 @@
       </c>
       <c r="N5" s="84">
         <f>$N$3</f>
-        <v>13</v>
+        <v>12.4789124008953</v>
       </c>
       <c r="O5" s="84">
         <v>12.341784891792569</v>
@@ -6963,7 +6963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -7936,99 +7936,99 @@
         <v>181</v>
       </c>
       <c r="G11" s="48">
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="H11" s="48">
         <f>$G$11</f>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="I11" s="48">
         <f t="shared" ref="I11:AD13" si="0">$G$11</f>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="J11" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="K11" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="L11" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="M11" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="N11" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="O11" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="P11" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Q11" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="R11" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="S11" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="T11" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="U11" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="V11" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="W11" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="X11" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Y11" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Z11" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AA11" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AB11" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AC11" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AD11" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AE11" s="48">
         <v>576</v>
@@ -8053,99 +8053,99 @@
       </c>
       <c r="G12" s="48">
         <f>$G$11</f>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="H12" s="48">
         <f t="shared" ref="H12" si="1">$G$11</f>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="I12" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="J12" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="K12" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="L12" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="M12" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="N12" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="O12" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="P12" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Q12" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="R12" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="S12" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="T12" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="U12" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="V12" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="W12" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="X12" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Y12" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Z12" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AA12" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AB12" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AC12" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AD12" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AE12" s="48">
         <v>648</v>
@@ -8166,99 +8166,99 @@
       </c>
       <c r="G13" s="48">
         <f t="shared" ref="G13:V16" si="2">$G$11</f>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="H13" s="48">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="I13" s="48">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="J13" s="48">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="K13" s="48">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="L13" s="48">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="M13" s="48">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="N13" s="48">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="O13" s="48">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="P13" s="48">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Q13" s="48">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="R13" s="48">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="S13" s="48">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="T13" s="48">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="U13" s="48">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="V13" s="48">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="W13" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="X13" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Y13" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Z13" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AA13" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AB13" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AC13" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AD13" s="48">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AE13" s="48"/>
       <c r="AF13" s="48"/>
@@ -8285,99 +8285,99 @@
       </c>
       <c r="G14" s="48">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="H14" s="48">
         <f t="shared" ref="H14:AD16" si="3">$G$11</f>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="I14" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="J14" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="K14" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="L14" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="M14" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="N14" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="O14" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="P14" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Q14" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="R14" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="S14" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="T14" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="U14" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="V14" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="W14" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="X14" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Y14" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Z14" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AA14" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AB14" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AC14" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AD14" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AE14" s="48">
         <v>504</v>
@@ -8402,99 +8402,99 @@
       </c>
       <c r="G15" s="48">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="H15" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="I15" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="J15" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="K15" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="L15" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="M15" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="N15" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="O15" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="P15" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Q15" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="R15" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="S15" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="T15" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="U15" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="V15" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="W15" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="X15" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Y15" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Z15" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AA15" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AB15" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AC15" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AD15" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AE15" s="48">
         <v>384</v>
@@ -8515,99 +8515,99 @@
       </c>
       <c r="G16" s="48">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="H16" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="I16" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="J16" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="K16" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="L16" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="M16" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="N16" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="O16" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="P16" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Q16" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="R16" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="S16" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="T16" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="U16" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="V16" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="W16" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="X16" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Y16" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Z16" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AA16" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AB16" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AC16" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AD16" s="48">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AE16" s="48">
         <v>384</v>
@@ -10015,99 +10015,99 @@
       </c>
       <c r="G32" s="48">
         <f>$G$11</f>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="H32" s="48">
         <f t="shared" ref="H32:AD37" si="4">$G$11</f>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="I32" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="J32" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="K32" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="L32" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="M32" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="N32" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="O32" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="P32" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Q32" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="R32" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="S32" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="T32" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="U32" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="V32" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="W32" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="X32" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Y32" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Z32" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AA32" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AB32" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AC32" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AD32" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AE32" s="48">
         <v>576</v>
@@ -10130,99 +10130,99 @@
       </c>
       <c r="G33" s="48">
         <f t="shared" ref="G33:G37" si="5">$G$11</f>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="H33" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="I33" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="J33" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="K33" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="L33" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="M33" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="N33" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="O33" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="P33" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Q33" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="R33" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="S33" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="T33" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="U33" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="V33" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="W33" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="X33" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Y33" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Z33" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AA33" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AB33" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AC33" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AD33" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AE33" s="48">
         <v>648</v>
@@ -10243,99 +10243,99 @@
       </c>
       <c r="G34" s="48">
         <f t="shared" si="5"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="H34" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="I34" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="J34" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="K34" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="L34" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="M34" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="N34" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="O34" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="P34" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Q34" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="R34" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="S34" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="T34" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="U34" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="V34" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="W34" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="X34" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Y34" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Z34" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AA34" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AB34" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AC34" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AD34" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AE34" s="48">
         <v>648</v>
@@ -10364,99 +10364,99 @@
       </c>
       <c r="G35" s="48">
         <f t="shared" si="5"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="H35" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="I35" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="J35" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="K35" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="L35" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="M35" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="N35" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="O35" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="P35" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Q35" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="R35" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="S35" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="T35" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="U35" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="V35" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="W35" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="X35" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Y35" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Z35" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AA35" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AB35" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AC35" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AD35" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AE35" s="48">
         <v>504</v>
@@ -10479,99 +10479,99 @@
       </c>
       <c r="G36" s="48">
         <f t="shared" si="5"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="H36" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="I36" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="J36" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="K36" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="L36" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="M36" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="N36" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="O36" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="P36" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Q36" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="R36" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="S36" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="T36" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="U36" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="V36" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="W36" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="X36" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Y36" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Z36" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AA36" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AB36" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AC36" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AD36" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AE36" s="48">
         <v>384</v>
@@ -10592,99 +10592,99 @@
       </c>
       <c r="G37" s="48">
         <f t="shared" si="5"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="H37" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="I37" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="J37" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="K37" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="L37" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="M37" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="N37" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="O37" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="P37" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Q37" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="R37" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="S37" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="T37" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="U37" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="V37" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="W37" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="X37" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Y37" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="Z37" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AA37" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AB37" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AC37" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AD37" s="48">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>23.356036669280886</v>
       </c>
       <c r="AE37" s="48">
         <v>384</v>

</xml_diff>

<commit_message>
Update result 4 and result 5 for surrogate-assited optimization
</commit_message>
<xml_diff>
--- a/data/DOERefBuildings/BLD10.xlsx
+++ b/data/DOERefBuildings/BLD10.xlsx
@@ -4413,13 +4413,13 @@
       <c r="K3" s="38"/>
       <c r="L3" s="38">
         <f>F3/L6</f>
-        <v>793.22902863825573</v>
+        <v>1177.6335921476248</v>
       </c>
       <c r="M3" s="84">
         <v>9.9</v>
       </c>
       <c r="N3" s="84">
-        <v>15.7818101893365</v>
+        <v>13.3965482697</v>
       </c>
       <c r="O3" s="84">
         <v>12.341784891792569</v>
@@ -4438,7 +4438,7 @@
       </c>
       <c r="T3" s="4"/>
       <c r="U3" s="84">
-        <v>0.53593736931288505</v>
+        <v>0.55866415655852553</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
@@ -4469,7 +4469,7 @@
       <c r="K4" s="38"/>
       <c r="L4" s="38">
         <f>$L$3</f>
-        <v>793.22902863825573</v>
+        <v>1177.6335921476248</v>
       </c>
       <c r="M4" s="84">
         <f>$M$3</f>
@@ -4477,7 +4477,7 @@
       </c>
       <c r="N4" s="84">
         <f>$N$3</f>
-        <v>15.7818101893365</v>
+        <v>13.3965482697</v>
       </c>
       <c r="O4" s="84">
         <v>12.341784891792569</v>
@@ -4498,7 +4498,7 @@
       <c r="T4" s="4"/>
       <c r="U4" s="84">
         <f>$U$3</f>
-        <v>0.53593736931288505</v>
+        <v>0.55866415655852553</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
@@ -4529,7 +4529,7 @@
       <c r="K5" s="38"/>
       <c r="L5" s="38">
         <f>$L$3</f>
-        <v>793.22902863825573</v>
+        <v>1177.6335921476248</v>
       </c>
       <c r="M5" s="84">
         <f>$M$3</f>
@@ -4537,7 +4537,7 @@
       </c>
       <c r="N5" s="84">
         <f>$N$3</f>
-        <v>15.7818101893365</v>
+        <v>13.3965482697</v>
       </c>
       <c r="O5" s="84">
         <v>12.341784891792569</v>
@@ -4558,12 +4558,12 @@
       <c r="T5" s="4"/>
       <c r="U5" s="84">
         <f>$U$3</f>
-        <v>0.53593736931288505</v>
+        <v>0.55866415655852553</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.15">
       <c r="L6">
-        <v>24.699045663562998</v>
+        <v>16.636753681822626</v>
       </c>
     </row>
   </sheetData>
@@ -5284,67 +5284,67 @@
         <v>486</v>
       </c>
       <c r="E12" s="66">
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="F12" s="66">
         <f>$E$12</f>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="G12" s="66">
         <f t="shared" ref="G12:T12" si="4">$E$12</f>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="H12" s="66">
         <f t="shared" si="4"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="I12" s="66">
         <f t="shared" si="4"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="J12" s="66">
         <f t="shared" si="4"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="K12" s="66">
         <f t="shared" si="4"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="L12" s="66">
         <f t="shared" si="4"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="M12" s="66">
         <f t="shared" si="4"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="N12" s="66">
         <f t="shared" si="4"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="O12" s="66">
         <f t="shared" si="4"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="P12" s="66">
         <f t="shared" si="4"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="Q12" s="66">
         <f t="shared" si="4"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="R12" s="66">
         <f t="shared" si="4"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="S12" s="66">
         <f t="shared" si="4"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="T12" s="66">
         <f t="shared" si="4"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="11.25" x14ac:dyDescent="0.15">
@@ -6024,67 +6024,67 @@
       </c>
       <c r="E23" s="66">
         <f>$E$12</f>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="F23" s="66">
         <f t="shared" ref="F23:T23" si="9">$E$12</f>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="G23" s="66">
         <f t="shared" si="9"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="H23" s="66">
         <f t="shared" si="9"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="I23" s="66">
         <f t="shared" si="9"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="J23" s="66">
         <f t="shared" si="9"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="K23" s="66">
         <f t="shared" si="9"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="L23" s="66">
         <f t="shared" si="9"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="M23" s="66">
         <f t="shared" si="9"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="N23" s="66">
         <f t="shared" si="9"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="O23" s="66">
         <f t="shared" si="9"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="P23" s="66">
         <f t="shared" si="9"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="Q23" s="66">
         <f t="shared" si="9"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="R23" s="66">
         <f t="shared" si="9"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="S23" s="66">
         <f t="shared" si="9"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="T23" s="66">
         <f t="shared" si="9"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
     </row>
     <row r="24" spans="1:20" ht="11.25" x14ac:dyDescent="0.15">
@@ -6764,67 +6764,67 @@
       </c>
       <c r="E34" s="66">
         <f>$E$12</f>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="F34" s="66">
         <f t="shared" ref="F34:T34" si="14">$E$12</f>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="G34" s="66">
         <f t="shared" si="14"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="H34" s="66">
         <f t="shared" si="14"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="I34" s="66">
         <f t="shared" si="14"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="J34" s="66">
         <f t="shared" si="14"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="K34" s="66">
         <f t="shared" si="14"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="L34" s="66">
         <f t="shared" si="14"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="M34" s="66">
         <f t="shared" si="14"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="N34" s="66">
         <f t="shared" si="14"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="O34" s="66">
         <f t="shared" si="14"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="P34" s="66">
         <f t="shared" si="14"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="Q34" s="66">
         <f t="shared" si="14"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="R34" s="66">
         <f t="shared" si="14"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="S34" s="66">
         <f t="shared" si="14"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
       <c r="T34" s="66">
         <f t="shared" si="14"/>
-        <v>3.2316396716731699</v>
+        <v>3.9660067703705058</v>
       </c>
     </row>
     <row r="35" spans="1:20" ht="11.25" x14ac:dyDescent="0.15">
@@ -7936,99 +7936,99 @@
         <v>181</v>
       </c>
       <c r="G11" s="48">
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="H11" s="48">
         <f>$G$11</f>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="I11" s="48">
         <f t="shared" ref="I11:AD13" si="0">$G$11</f>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="J11" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="K11" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="L11" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="M11" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="N11" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="O11" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="P11" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Q11" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="R11" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="S11" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="T11" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="U11" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="V11" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="W11" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="X11" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Y11" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Z11" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AA11" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AB11" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AC11" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AD11" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AE11" s="48">
         <v>576</v>
@@ -8053,99 +8053,99 @@
       </c>
       <c r="G12" s="48">
         <f>$G$11</f>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="H12" s="48">
         <f t="shared" ref="H12" si="1">$G$11</f>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="I12" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="J12" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="K12" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="L12" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="M12" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="N12" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="O12" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="P12" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Q12" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="R12" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="S12" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="T12" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="U12" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="V12" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="W12" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="X12" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Y12" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Z12" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AA12" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AB12" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AC12" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AD12" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AE12" s="48">
         <v>648</v>
@@ -8166,99 +8166,99 @@
       </c>
       <c r="G13" s="48">
         <f t="shared" ref="G13:V16" si="2">$G$11</f>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="H13" s="48">
         <f t="shared" si="2"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="I13" s="48">
         <f t="shared" si="2"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="J13" s="48">
         <f t="shared" si="2"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="K13" s="48">
         <f t="shared" si="2"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="L13" s="48">
         <f t="shared" si="2"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="M13" s="48">
         <f t="shared" si="2"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="N13" s="48">
         <f t="shared" si="2"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="O13" s="48">
         <f t="shared" si="2"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="P13" s="48">
         <f t="shared" si="2"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Q13" s="48">
         <f t="shared" si="2"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="R13" s="48">
         <f t="shared" si="2"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="S13" s="48">
         <f t="shared" si="2"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="T13" s="48">
         <f t="shared" si="2"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="U13" s="48">
         <f t="shared" si="2"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="V13" s="48">
         <f t="shared" si="2"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="W13" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="X13" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Y13" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Z13" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AA13" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AB13" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AC13" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AD13" s="48">
         <f t="shared" si="0"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AE13" s="48"/>
       <c r="AF13" s="48"/>
@@ -8285,99 +8285,99 @@
       </c>
       <c r="G14" s="48">
         <f t="shared" si="2"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="H14" s="48">
         <f t="shared" ref="H14:AD16" si="3">$G$11</f>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="I14" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="J14" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="K14" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="L14" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="M14" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="N14" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="O14" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="P14" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Q14" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="R14" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="S14" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="T14" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="U14" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="V14" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="W14" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="X14" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Y14" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Z14" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AA14" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AB14" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AC14" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AD14" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AE14" s="48">
         <v>504</v>
@@ -8402,99 +8402,99 @@
       </c>
       <c r="G15" s="48">
         <f t="shared" si="2"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="H15" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="I15" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="J15" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="K15" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="L15" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="M15" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="N15" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="O15" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="P15" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Q15" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="R15" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="S15" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="T15" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="U15" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="V15" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="W15" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="X15" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Y15" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Z15" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AA15" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AB15" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AC15" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AD15" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AE15" s="48">
         <v>384</v>
@@ -8515,99 +8515,99 @@
       </c>
       <c r="G16" s="48">
         <f t="shared" si="2"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="H16" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="I16" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="J16" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="K16" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="L16" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="M16" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="N16" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="O16" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="P16" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Q16" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="R16" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="S16" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="T16" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="U16" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="V16" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="W16" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="X16" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Y16" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Z16" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AA16" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AB16" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AC16" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AD16" s="48">
         <f t="shared" si="3"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AE16" s="48">
         <v>384</v>
@@ -10015,99 +10015,99 @@
       </c>
       <c r="G32" s="48">
         <f>$G$11</f>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="H32" s="48">
         <f t="shared" ref="H32:AD37" si="4">$G$11</f>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="I32" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="J32" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="K32" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="L32" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="M32" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="N32" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="O32" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="P32" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Q32" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="R32" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="S32" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="T32" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="U32" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="V32" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="W32" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="X32" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Y32" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Z32" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AA32" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AB32" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AC32" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AD32" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AE32" s="48">
         <v>576</v>
@@ -10130,99 +10130,99 @@
       </c>
       <c r="G33" s="48">
         <f t="shared" ref="G33:G37" si="5">$G$11</f>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="H33" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="I33" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="J33" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="K33" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="L33" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="M33" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="N33" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="O33" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="P33" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Q33" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="R33" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="S33" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="T33" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="U33" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="V33" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="W33" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="X33" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Y33" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Z33" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AA33" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AB33" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AC33" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AD33" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AE33" s="48">
         <v>648</v>
@@ -10243,99 +10243,99 @@
       </c>
       <c r="G34" s="48">
         <f t="shared" si="5"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="H34" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="I34" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="J34" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="K34" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="L34" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="M34" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="N34" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="O34" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="P34" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Q34" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="R34" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="S34" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="T34" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="U34" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="V34" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="W34" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="X34" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Y34" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Z34" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AA34" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AB34" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AC34" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AD34" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AE34" s="48">
         <v>648</v>
@@ -10364,99 +10364,99 @@
       </c>
       <c r="G35" s="48">
         <f t="shared" si="5"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="H35" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="I35" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="J35" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="K35" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="L35" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="M35" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="N35" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="O35" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="P35" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Q35" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="R35" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="S35" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="T35" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="U35" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="V35" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="W35" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="X35" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Y35" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Z35" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AA35" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AB35" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AC35" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AD35" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AE35" s="48">
         <v>504</v>
@@ -10479,99 +10479,99 @@
       </c>
       <c r="G36" s="48">
         <f t="shared" si="5"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="H36" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="I36" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="J36" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="K36" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="L36" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="M36" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="N36" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="O36" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="P36" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Q36" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="R36" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="S36" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="T36" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="U36" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="V36" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="W36" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="X36" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Y36" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Z36" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AA36" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AB36" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AC36" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AD36" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AE36" s="48">
         <v>384</v>
@@ -10592,99 +10592,99 @@
       </c>
       <c r="G37" s="48">
         <f t="shared" si="5"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="H37" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="I37" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="J37" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="K37" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="L37" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="M37" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="N37" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="O37" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="P37" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Q37" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="R37" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="S37" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="T37" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="U37" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="V37" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="W37" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="X37" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Y37" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="Z37" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AA37" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AB37" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AC37" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AD37" s="48">
         <f t="shared" si="4"/>
-        <v>23.506754202891202</v>
+        <v>23.130357207884092</v>
       </c>
       <c r="AE37" s="48">
         <v>384</v>

</xml_diff>